<commit_message>
Revert "rehab 2.1.1 added"
This reverts commit 29fce63a26de094ccef2bfa3ffa40d6d80d3c21e.
</commit_message>
<xml_diff>
--- a/rehab/StructureDefinition-BasedOnCarePlanExtension.xlsx
+++ b/rehab/StructureDefinition-BasedOnCarePlanExtension.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>2.1.1</t>
+    <t>2.1.0</t>
   </si>
   <si>
     <t>Name</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-06-24T12:49:29+02:00</t>
+    <t>2024-06-19T13:11:07+02:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>